<commit_message>
Update with CORS fix and latest deployment logic
</commit_message>
<xml_diff>
--- a/submissions/submissions.xlsx
+++ b/submissions/submissions.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -470,6 +470,43 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Daniel </t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2002-04-25</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>(917) 975-2625</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>dshifrin5@gmail.com</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>1181</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>www</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>2025-05-27 21-43-00</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
WIP: Local changes before pull
</commit_message>
<xml_diff>
--- a/submissions/submissions.xlsx
+++ b/submissions/submissions.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -507,6 +507,202 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2025-05-28 21-11-13</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Daniel </t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>2000-01-01</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>(917) 975-2625</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>dshifrin5@gmail.com</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>1181</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>141</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2025-05-28 21-20-50</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Daniel Shifrin</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>2002-04-25</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>9179752625</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>dshifrin@sandiego.edu</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>1181</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Check up</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2025-05-28 21-37-01</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Daniel Shifrin</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>2002-04-25</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>(917) 975-2625</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>dshifrin5@gmail.com</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>1181</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Checkup</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2025-05-28 21-48-14</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Daniel </t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>2013-12-31</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>9179752625</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>dshifrin5@gmail.com</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>1181</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>ygtu</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2025-05-29 23-09-44</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>robert99023@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2025-05-29 23-09-45</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>robert99023@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2025-05-29 23-17-34</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>elizavetakutko@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2025-05-29 23-17-35</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>elizavetakutko@gmail.com</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>